<commit_message>
Implement advanced cascade delete with hierarchical dependency visualization
- Add hierarchical tree-view for displaying related records before deletion
- Implement drill-down capability to explore nested dependencies
- Add configurable field display per object type for better context
- Create transaction-based cascade delete with automatic rollback
- Replace all toast notifications with modal dialogs
- Add progress tracking for multi-record delete operations
- Fix ProductClassification dependency detection
- Update documentation with new delete functionality
- Enhance error handling with plain English messages and suggested fixes

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/templates/master/Revenue_Cloud_Complete_Upload_Template.xlsx
+++ b/data/templates/master/Revenue_Cloud_Complete_Upload_Template.xlsx
@@ -43,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -128,6 +128,9 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -155,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -422,12 +425,18 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -524,6 +533,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7483,144 +7495,144 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="18.33203125" bestFit="1" customWidth="1" style="51" min="1" max="1"/>
-    <col width="24.83203125" customWidth="1" style="51" min="2" max="2"/>
-    <col width="10" bestFit="1" customWidth="1" style="51" min="3" max="3"/>
-    <col width="22.5" bestFit="1" customWidth="1" style="51" min="4" max="4"/>
-    <col width="10.5" bestFit="1" customWidth="1" style="51" min="5" max="5"/>
-    <col width="17.6640625" bestFit="1" customWidth="1" style="51" min="6" max="6"/>
-    <col width="14.33203125" bestFit="1" customWidth="1" style="51" min="7" max="7"/>
-    <col width="17.33203125" bestFit="1" customWidth="1" style="51" min="8" max="8"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="52" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="52" t="inlineStr">
         <is>
           <t>CatalogType</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="52" t="inlineStr">
         <is>
           <t>EffectiveStartDate</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="52" t="inlineStr">
         <is>
           <t>EffectiveEndDate</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>AB Test Catalog</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="2" t="n"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0ZSdp00000007kfGAA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cyber</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cyber</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cyber Products</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-06-02T00:00:00.000+0000</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007nzGAA</t>
-        </is>
-      </c>
-      <c r="B3" s="20" t="inlineStr">
-        <is>
-          <t>AB Test Catalog</t>
-        </is>
-      </c>
-      <c r="C3" s="20" t="n"/>
-      <c r="D3" s="20" t="n"/>
-      <c r="E3" s="20" t="n"/>
-      <c r="F3" s="21" t="n"/>
-      <c r="G3" s="20" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0ZSdp00000007kgGAA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Tech Products</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-03T00:00:00.000+0000</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kfGAA</t>
-        </is>
-      </c>
-      <c r="B4" s="13" t="inlineStr">
-        <is>
-          <t>Cyber</t>
-        </is>
-      </c>
-      <c r="C4" s="13" t="inlineStr">
-        <is>
-          <t>Cyber</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>Cyber products.</t>
-        </is>
-      </c>
-      <c r="E4" s="13" t="n"/>
-      <c r="F4" s="13" t="n"/>
-      <c r="G4" s="13" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kgGAA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Tech products.</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0ZSdp0000000ASPGA2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Corporate</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Corp</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Corporate Products</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sales</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7758,43 +7770,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>External_ID__c*</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status*</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>BillingTreatmentSelection*</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1BPdp0000006WbVGAU</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Billing Policy</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7804,53 +7813,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>External_ID__c*</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>BillingPolicy.External_ID__c</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status*</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntity.External_ID__c</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ExcludeFromBilling*</t>
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1BTdp0000000ITBGA2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Fortra Billing Treatment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7860,75 +7856,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="14.1640625" bestFit="1" customWidth="1" style="51" min="1" max="1"/>
-    <col width="14.5" bestFit="1" customWidth="1" style="51" min="2" max="2"/>
-    <col width="13.6640625" bestFit="1" customWidth="1" style="51" min="3" max="3"/>
-    <col width="14.33203125" bestFit="1" customWidth="1" style="51" min="4" max="4"/>
-    <col width="5.83203125" bestFit="1" customWidth="1" style="51" min="5" max="5"/>
-    <col width="14.5" bestFit="1" customWidth="1" style="51" min="6" max="6"/>
-    <col width="12.6640625" bestFit="1" customWidth="1" style="51" min="7" max="7"/>
-    <col width="13.6640625" bestFit="1" customWidth="1" style="51" min="8" max="8"/>
-    <col width="18.5" bestFit="1" customWidth="1" style="51" min="9" max="9"/>
-    <col width="15.83203125" bestFit="1" customWidth="1" style="51" min="10" max="10"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>CompanyName</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntityStreet</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntityCity</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntityState</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntityPostalCode</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>LegalEntityCountry</t>
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0fwdp0000000DuvAAE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Fortra</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7938,43 +7899,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TaxCode</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>IsTaxable*</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Status*</t>
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1ttdp0000000IZdAAM</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Fortra Tax Treatment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7984,38 +7942,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Status*</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TreatmentSelection*</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1Tpdp0000000GZRCA2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Fortra Tax Policy</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8025,68 +7985,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEngineName*</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status*</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SellerCode</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEngineStreet</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEngineCity</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEngineState</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEnginePostalCode</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>TaxEngineCountry</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8096,1287 +8003,76 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="19.6640625" bestFit="1" customWidth="1" style="51" min="1" max="1"/>
-    <col width="21.6640625" customWidth="1" style="51" min="2" max="2"/>
-    <col width="10.83203125" customWidth="1" style="51" min="3" max="3"/>
-    <col width="19.6640625" bestFit="1" customWidth="1" style="51" min="4" max="4"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>CatalogId</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>SortOrder</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0ZGdp00000007JFGAY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Core Offerings</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0ZGdp00000007JGGAY</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Add-Ons</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0ZGdp00000007JHGAY</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Standalone</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="20" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="B5" s="20" t="n"/>
-      <c r="C5" s="20" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="D5" s="20" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="n"/>
-      <c r="C6" s="13" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-      <c r="D6" s="13" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>AB Test Category</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007mHGAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Core Offerings</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kfGAA</t>
-        </is>
-      </c>
-      <c r="D98" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0ZGdp00000007JIGAY</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Bundle Components</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>BC</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kfGAA</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Add-Ons</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>AO</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kfGAA</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>Standalone</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>0ZSdp00000007kfGAA</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -12625,203 +11321,167 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col width="20.83203125" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="24.5" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="13.33203125" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="6.1640625" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="10.83203125" customWidth="1" style="6" min="5" max="22"/>
-    <col width="10.83203125" customWidth="1" style="6" min="23" max="16384"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="52" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>11Bdp000000nAELEA2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Product Attributes</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PROD_ATTRS</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>11Bdp000000nBLhEAM</t>
         </is>
       </c>
-      <c r="B2" s="18" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Data Protection</t>
         </is>
       </c>
-      <c r="C2" s="18" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>DP</t>
         </is>
       </c>
-      <c r="D2" s="7" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>11Bdp000000nBLiEAM</t>
         </is>
       </c>
-      <c r="B3" s="18" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Defensive Security Solutions</t>
         </is>
       </c>
-      <c r="C3" s="18" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>DSS</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="inlineStr">
-        <is>
-          <t>11Bdp000000nBLjEAM</t>
-        </is>
-      </c>
-      <c r="B4" s="18" t="inlineStr">
-        <is>
-          <t>IBM I Security</t>
-        </is>
-      </c>
-      <c r="C4" s="18" t="inlineStr">
-        <is>
-          <t>IIS</t>
-        </is>
-      </c>
-      <c r="D4" s="7" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11Bdp000000nBLkEAM</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Managed Security Services</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MSS</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11Bdp000000nBLlEAM</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Offensive Security Solutions</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OSPM</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="inlineStr">
-        <is>
-          <t>11Bdp000000nBLkEAM</t>
-        </is>
-      </c>
-      <c r="B5" s="18" t="inlineStr">
-        <is>
-          <t>Managed Security Services</t>
-        </is>
-      </c>
-      <c r="C5" s="18" t="inlineStr">
-        <is>
-          <t>MSS</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11Bdp000000sVd7EAE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Human Risk Management</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>HMR</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="inlineStr">
-        <is>
-          <t>11Bdp000000nBLlEAM</t>
-        </is>
-      </c>
-      <c r="B6" s="18" t="inlineStr">
-        <is>
-          <t>Offensive Security Solutions</t>
-        </is>
-      </c>
-      <c r="C6" s="18" t="inlineStr">
-        <is>
-          <t>OSPM</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="inlineStr">
-        <is>
-          <t>11Bdp000000nAELEA2</t>
-        </is>
-      </c>
-      <c r="B7" s="18" t="inlineStr">
-        <is>
-          <t>Product Attributes</t>
-        </is>
-      </c>
-      <c r="C7" s="18" t="inlineStr">
-        <is>
-          <t>PROD_ATTRS</t>
-        </is>
-      </c>
-      <c r="D7" s="7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
-        <is>
-          <t>11Bdp000000nBLmEAM</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>Secure File Transfer</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="inlineStr">
-        <is>
-          <t>SFT</t>
-        </is>
-      </c>
-      <c r="D8" s="7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="n"/>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="7" t="n"/>
-      <c r="D9" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix bundle component display issues in Product Hierarchy
- Fixed DCS bundle ID mismatch in server.py (old IDs -> new JEG* IDs)
- Fixed component column positioning formula in product-hierarchy.html
- Added bundle-component relationships to Excel workbook
- All 6 bundles (3 DCS + 3 HRM) now correctly display their components

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/templates/master/Revenue_Cloud_Complete_Upload_Template.xlsx
+++ b/data/templates/master/Revenue_Cloud_Complete_Upload_Template.xlsx
@@ -5366,7 +5366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5485,68 +5485,6 @@
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>0ZSdp0000000BBZGA2</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Test3</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>TEST3</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>sadfsadf</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Sales</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>2025-07-01T13:46:00.000+0000</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>0ZSdp0000000BDBGA2</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Testx</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>TESTX</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr"/>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>Sales</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>2025-07-03T13:59:00.000+0000</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7605,7 +7543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7615,7 +7553,7 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="42" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
     <col width="33" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
@@ -9977,6 +9915,132 @@
       <c r="Q37" s="3" t="inlineStr"/>
       <c r="R37" s="3" t="inlineStr"/>
     </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006tQw5AAE</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="inlineStr"/>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3" t="inlineStr"/>
+      <c r="H38" s="3" t="inlineStr"/>
+      <c r="I38" s="3" t="inlineStr"/>
+      <c r="J38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" s="3" t="inlineStr"/>
+      <c r="L38" s="3" t="inlineStr"/>
+      <c r="M38" s="3" t="inlineStr"/>
+      <c r="N38" s="3" t="inlineStr"/>
+      <c r="O38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3" t="inlineStr"/>
+      <c r="Q38" s="3" t="inlineStr"/>
+      <c r="R38" s="3" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006tdZxAAI</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>Manual Test Product 20250728_141722</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>TEST_MANUAL_1753730242</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr"/>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>Manual test product</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="inlineStr"/>
+      <c r="H39" s="3" t="inlineStr"/>
+      <c r="I39" s="3" t="inlineStr"/>
+      <c r="J39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3" t="inlineStr"/>
+      <c r="L39" s="3" t="inlineStr"/>
+      <c r="M39" s="3" t="inlineStr"/>
+      <c r="N39" s="3" t="inlineStr"/>
+      <c r="O39" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3" t="inlineStr"/>
+      <c r="Q39" s="3" t="inlineStr"/>
+      <c r="R39" s="3" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006tgb3AAA</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>Test Product</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>TEST_PRODUCT</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr"/>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>kujh</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="inlineStr"/>
+      <c r="H40" s="3" t="inlineStr"/>
+      <c r="I40" s="3" t="inlineStr"/>
+      <c r="J40" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3" t="inlineStr"/>
+      <c r="L40" s="3" t="inlineStr"/>
+      <c r="M40" s="3" t="inlineStr"/>
+      <c r="N40" s="3" t="inlineStr"/>
+      <c r="O40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3" t="inlineStr"/>
+      <c r="Q40" s="3" t="inlineStr"/>
+      <c r="R40" s="3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9988,7 +10052,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9997,7 +10061,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="6" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10008,7 +10073,12 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>ProductId</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>ProductCategoryId</t>
         </is>
       </c>
     </row>
@@ -10018,8 +10088,15 @@
           <t>0ZRdp0000000DwXGAU</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>174</v>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006JEGkAAO</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000Ax3GAE</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -10028,8 +10105,15 @@
           <t>0ZRdp0000000Dy9GAE</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>178</v>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006JEGjAAO</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000Ax3GAE</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -10038,8 +10122,15 @@
           <t>0ZRdp0000000DyAGAU</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>179</v>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006JEGlAAO</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000Ax3GAE</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -10048,8 +10139,15 @@
           <t>0ZRdp0000000DzlGAE</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>181</v>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006iLGbAAM</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AyfGAE</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -10058,8 +10156,15 @@
           <t>0ZRdp0000000E6DGAU</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>188</v>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006m0jpAAA</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AyfGAE</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -10068,8 +10173,66 @@
           <t>0ZRdp0000000E7pGAE</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>189</v>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006m14nAAA</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AyfGAE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>0ZRdp0000000EFtGAM</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006tcR0AAI</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AqbGAE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>0ZRdp0000000EHVGA2</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006teFtAAI</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AqbGAE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>0ZRdp0000000EJ7GAM</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>01tdp000006tfiDAAQ</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>0ZGdp0000000AqbGAE</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>